<commit_message>
added excel for exportar ult estado
</commit_message>
<xml_diff>
--- a/static/excel/exportar_ult_estado.xlsx
+++ b/static/excel/exportar_ult_estado.xlsx
@@ -47,9 +47,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$$-2C0A]#,##0.00;[RED]\([$$-2C0A]#,##0.00\)"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -135,17 +134,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -331,23 +326,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A9:G49"/>
+  <dimension ref="A9:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.79"/>
   </cols>
   <sheetData>
-    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -369,162 +363,6 @@
       <c r="G9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>